<commit_message>
Figures made for next update for co-authors, about Random forest + PLSR + Spearman correlations
</commit_message>
<xml_diff>
--- a/MostImportantCHCs.xlsx
+++ b/MostImportantCHCs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\0 - R\Ant-CHCs-Desiccation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22251A68-1049-4D51-B2DD-413E573D1332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86385DCF-EF2C-484E-A81B-EE8275F9FB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14310" yWindow="12420" windowWidth="12390" windowHeight="11790" tabRatio="634" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="634" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 8 CHCs (df1)" sheetId="3" r:id="rId1"/>
@@ -384,7 +384,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>IncNodePurity</t>
   </si>
@@ -618,6 +618,12 @@
   </si>
   <si>
     <t>PLSR.LWS</t>
+  </si>
+  <si>
+    <t>(Using raw CHC mass estimates)</t>
+  </si>
+  <si>
+    <t>(Using "CHC mass per body mass")</t>
   </si>
 </sst>
 </file>
@@ -1486,7 +1492,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,6 +1685,11 @@
         <v>-0.163522</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
@@ -1694,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,6 +1899,11 @@
       </c>
       <c r="F9">
         <v>-0.17247100000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>